<commit_message>
Vou melhorar o modulo da gravação
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Tarefa</t>
   </si>
@@ -424,39 +424,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -469,6 +436,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -478,7 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +783,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B18" sqref="B18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,12 +797,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="17" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -813,7 +813,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -858,259 +858,285 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="18" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="29" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="24" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="24" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="24" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="24" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="24" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="24" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="24" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="24" t="s">
-        <v>19</v>
+      <c r="C18" s="20"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="22"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="22"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="22"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="22"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="22"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="22"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="22"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="22"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="22"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="22"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="22"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="22"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="22"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="22"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="22"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="22"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="22"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="22"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="22"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="10"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="23"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
@@ -1118,30 +1144,6 @@
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>

<commit_message>
Teste normal modo aluno, que terá de ser ligada com a pasta da escolha das categorias
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Folha2" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Tarefa</t>
   </si>
@@ -84,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +437,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -444,39 +477,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -494,7 +494,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -568,7 +568,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -603,7 +602,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -779,14 +777,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
@@ -795,13 +793,13 @@
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -809,7 +807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="15.75" hidden="1" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -817,7 +815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="15.75" hidden="1" thickBot="1">
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -825,7 +823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="15.75" hidden="1" thickBot="1">
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -833,7 +831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="15.75" hidden="1" thickBot="1">
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -841,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="15.75" hidden="1" thickBot="1">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -849,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="15.75" hidden="1" thickBot="1">
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -857,12 +855,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="7" t="s">
         <v>2</v>
       </c>
@@ -870,100 +868,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="8"/>
       <c r="F10" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+    <row r="11" spans="2:6">
+      <c r="B11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="7"/>
       <c r="F11" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+    <row r="12" spans="2:6">
+      <c r="B12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="8"/>
       <c r="F12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+    <row r="13" spans="2:6">
+      <c r="B13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="7"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F13" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="2:6">
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="8"/>
       <c r="F14" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+    <row r="15" spans="2:6">
+      <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="7"/>
       <c r="F15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+    <row r="16" spans="2:6" ht="17.25" customHeight="1">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+    <row r="17" spans="2:6" ht="27.75" customHeight="1">
+      <c r="B17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="7"/>
       <c r="F17" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="8" t="s">
         <v>5</v>
       </c>
@@ -971,148 +971,167 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+    <row r="19" spans="2:6">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="7"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
+    <row r="20" spans="2:6">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="7"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
+    <row r="21" spans="2:6">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="7"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
+    <row r="22" spans="2:6">
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="7"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
+    <row r="23" spans="2:6">
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="7"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
+    <row r="24" spans="2:6">
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="7"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
+    <row r="25" spans="2:6">
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="7"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+    <row r="26" spans="2:6">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="7"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
+    <row r="27" spans="2:6">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="7"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
+    <row r="28" spans="2:6">
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="7"/>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
+    <row r="29" spans="2:6">
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="7"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
+    <row r="30" spans="2:6">
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="7"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="21"/>
+    <row r="31" spans="2:6">
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="8"/>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="21"/>
+    <row r="32" spans="2:6">
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="7"/>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="21"/>
+    <row r="33" spans="2:6">
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="8"/>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
+    <row r="34" spans="2:6">
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="7"/>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="21"/>
+    <row r="35" spans="2:6">
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="8"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
+    <row r="36" spans="2:6">
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="7"/>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
+    <row r="37" spans="2:6">
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="9"/>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+    <row r="38" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29"/>
       <c r="E38" s="10"/>
       <c r="F38" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
@@ -1125,25 +1144,6 @@
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>
@@ -1151,24 +1151,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testes modo aluno, que terão de ser posteriormente ligados com a página da escolha de categoria
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -781,7 +781,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -910,8 +910,8 @@
       <c r="E13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>19</v>
+      <c r="F13" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:6">

</xml_diff>

<commit_message>
Uma tarefa feita, outra a ser feita
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Tarefa</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>A fazer..</t>
+  </si>
+  <si>
+    <t>Feito</t>
   </si>
 </sst>
 </file>
@@ -102,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +124,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -418,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -437,6 +446,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -783,7 +793,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,11 +807,11 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -858,11 +868,11 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="7" t="s">
         <v>2</v>
       </c>
@@ -871,33 +881,33 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="8"/>
       <c r="F10" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="7"/>
       <c r="F11" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="8" t="s">
         <v>4</v>
       </c>
@@ -906,11 +916,11 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="7" t="s">
         <v>3</v>
       </c>
@@ -919,199 +929,201 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="8"/>
       <c r="F14" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="7"/>
       <c r="F15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="13" t="s">
-        <v>19</v>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="7"/>
       <c r="F17" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>20</v>
+      <c r="F18" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="7"/>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="7"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="7"/>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="7"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="7"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="7"/>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="7"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="7"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="7"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="7"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="7"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="7"/>
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="8"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="21"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="7"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="8"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="7"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="8"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="7"/>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="9"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="10"/>
       <c r="F38" s="12"/>
     </row>

</xml_diff>

<commit_message>
Realização de um ecra de teste para o aluno. O teste será efectuado através de uma associação de um teste a uma imagem
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Tarefa</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Feito</t>
+  </si>
+  <si>
+    <t>A fazer...</t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,9 +900,11 @@
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="13" t="s">
-        <v>19</v>
+      <c r="E11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -945,9 +950,11 @@
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="13" t="s">
-        <v>19</v>
+      <c r="E15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A Tarefa de ligação ao servidor e download dos testes já foi implementada pelo grupo de Sistemas de Informação. Eu estou a enviar a actualização do Excel.
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Tarefa</t>
   </si>
@@ -85,13 +85,46 @@
   </si>
   <si>
     <t>A fazer...</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nota:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feito pelo grupo de Sistemas de Informação. Se forem ao github "letrinhas_si" encontram lá</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +136,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -275,7 +323,136 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -290,7 +467,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -299,26 +476,24 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -327,97 +502,14 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -430,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -441,56 +533,79 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,6 +616,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -549,7 +667,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,7 +702,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F38"/>
+  <dimension ref="B1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,13 +926,13 @@
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -822,7 +940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -830,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -838,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -846,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -854,7 +972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -862,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -870,12 +988,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="7" t="s">
         <v>2</v>
       </c>
@@ -883,36 +1001,46 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="37"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="8" t="s">
         <v>4</v>
       </c>
@@ -920,12 +1048,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="7" t="s">
         <v>3</v>
       </c>
@@ -933,23 +1061,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
@@ -957,12 +1087,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="8" t="s">
         <v>5</v>
       </c>
@@ -971,171 +1101,192 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="7"/>
       <c r="F17" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="7"/>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="7"/>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="7"/>
       <c r="F21" s="11"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="7"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="7"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="7"/>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="7"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="7"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="7"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="7"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="7"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="7"/>
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="8"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="7"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="8"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="7"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="8"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="22"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="7"/>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="22"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="9"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29"/>
       <c r="E38" s="10"/>
       <c r="F38" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="33">
+    <mergeCell ref="G10:K11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
@@ -1148,25 +1299,6 @@
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>

<commit_message>
Continuação da pagina Teste de Texto, e update de mais algumas imagens!
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>Tarefa</t>
   </si>
@@ -48,15 +48,6 @@
     <t>Fazer o pedido do teste e recebe-lo (online)</t>
   </si>
   <si>
-    <t>Executar o teste normal (offline) modo de professor</t>
-  </si>
-  <si>
-    <t>Executar o teste com imagens (offline) modo aluno</t>
-  </si>
-  <si>
-    <t>Executar o teste com imagens (offline) modo professor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enviar os resultados (voz e classificação) para o servidor, sugiro que este se faça sempre que exista resultados no tablet. </t>
   </si>
   <si>
@@ -72,9 +63,6 @@
     <t>Por fazer</t>
   </si>
   <si>
-    <t>A fazer..</t>
-  </si>
-  <si>
     <t>Feito</t>
   </si>
   <si>
@@ -84,30 +72,15 @@
     <t>Guardar / extrair os dados (texto, imagens, som) da Base de dados (SQlight), no android</t>
   </si>
   <si>
-    <t>Sincronização com o SI</t>
-  </si>
-  <si>
-    <t>12.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Detetar se existe rede (WI-FI/3G/GSM) </t>
   </si>
   <si>
-    <t>12.3</t>
-  </si>
-  <si>
     <t>Replicar as BD's dos professores e dos alunos de acordo com o agrupamento</t>
   </si>
   <si>
-    <t>12.4</t>
-  </si>
-  <si>
     <t>Sincronizar as bd's de 12.3</t>
   </si>
   <si>
-    <t>Escolher os testes a realizar (ano/area/testes)</t>
-  </si>
-  <si>
     <t>Guardar os testes na Bd Andorid</t>
   </si>
   <si>
@@ -117,36 +90,18 @@
     <t>13.1</t>
   </si>
   <si>
-    <t>13.2</t>
-  </si>
-  <si>
-    <t>13.3</t>
-  </si>
-  <si>
     <t>Realizar um teste</t>
   </si>
   <si>
-    <t>sincronizar o resultado do teste c/ o servidor</t>
-  </si>
-  <si>
-    <t>13.4</t>
-  </si>
-  <si>
     <t>Estatísticas do aluno</t>
   </si>
   <si>
     <t>V0.3</t>
   </si>
   <si>
-    <t>Desenvolver uma classe para o calculo dos parametros de avaliação</t>
-  </si>
-  <si>
     <t>Ecrãs de autenticação</t>
   </si>
   <si>
-    <t xml:space="preserve">17.1 </t>
-  </si>
-  <si>
     <t>ecrãs dinâmicos com botões de imagens (alunos / testes /professores)</t>
   </si>
   <si>
@@ -159,12 +114,6 @@
     <t>opcional</t>
   </si>
   <si>
-    <t xml:space="preserve">Executar o teste normal (offline) modo de aluno, pagina única. </t>
-  </si>
-  <si>
-    <t>Analisar</t>
-  </si>
-  <si>
     <t>barra / ampulheta de tempo a decorrer.. (Professor)</t>
   </si>
   <si>
@@ -172,9 +121,6 @@
   </si>
   <si>
     <t>Resultados dos testes:</t>
-  </si>
-  <si>
-    <t>15.1</t>
   </si>
   <si>
     <r>
@@ -199,6 +145,48 @@
   </si>
   <si>
     <t>V0.4</t>
+  </si>
+  <si>
+    <t>Executar o teste de Texto em modo de aluno / modo de professor</t>
+  </si>
+  <si>
+    <t>Executar o teste de Palavras em modo de aluno / modo de professor</t>
+  </si>
+  <si>
+    <t>Executar o teste de Poemas em modo de aluno / modo de professor</t>
+  </si>
+  <si>
+    <t>Executar o teste de Compreenção (Imagens) em modo de aluno / modo de professor</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>Escolher o tema dos testes a realizar (ano/area/testes)</t>
+  </si>
+  <si>
+    <t>Sincronização com o SI:</t>
+  </si>
+  <si>
+    <t>Desenvolver uma classe para apoio no calculo dos parametros de avaliação</t>
   </si>
 </sst>
 </file>
@@ -222,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,8 +247,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -580,11 +574,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -595,7 +604,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -616,13 +624,63 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,66 +708,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="B25" sqref="B25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,20 +1041,21 @@
     <col min="3" max="3" width="35.42578125" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1092,48 +1107,46 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="22">
         <v>1</v>
       </c>
-      <c r="B9" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="7" t="s">
+      <c r="B9" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>18</v>
+      <c r="F9" s="60" t="s">
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="22">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>19</v>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>48</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="H10" s="45"/>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="22">
         <v>3</v>
       </c>
       <c r="B11" s="42" t="s">
@@ -1141,502 +1154,457 @@
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="44"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="15" t="s">
-        <v>19</v>
+      <c r="E11" s="47"/>
+      <c r="F11" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="30"/>
+        <v>29</v>
+      </c>
+      <c r="H11" s="45"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="22">
         <v>4</v>
       </c>
-      <c r="B12" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="B12" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="59"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="25">
         <v>5</v>
       </c>
-      <c r="B13" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>18</v>
+      <c r="B13" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="61"/>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>7</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="61"/>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>8</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
+        <v>9</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
         <v>10</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="14" t="s">
+      <c r="B18" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="61"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" s="45" t="s">
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
         <v>11</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
-        <v>8</v>
-      </c>
-      <c r="B16" s="48" t="s">
+      <c r="B22" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="61"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
         <v>12</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="13" t="s">
+      <c r="B27" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="18">
+        <v>13</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="61"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="22">
+        <v>14</v>
+      </c>
+      <c r="B30" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <v>15</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="22">
+        <v>16</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>17</v>
       </c>
-      <c r="G16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24">
-        <v>10</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>12</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
-        <v>13</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B33" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="21">
-        <v>14</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="45"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
-        <v>15</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>16</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>17</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>18</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="18"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="28"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="9"/>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="45"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="12"/>
-    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="29">
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>

<commit_message>
Update - Modulo de avaliação, concluído, limar a app para se porder apresentar qualquer coisa, e não passar tanta vergonha! Vou arrancar para a interação com a BD local e retirar o seu conteúdo para preencher os testes...
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Folha2" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Tarefa</t>
   </si>
@@ -216,10 +216,7 @@
     <t>Implementar a gravação de voz no teste e implemntar e  a selecção das palavras erradas no texto.</t>
   </si>
   <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>Apresentar relatório da avaliação no fim de correr todos os testes escolhidos</t>
+    <t>Apresentar relatório da avaliação no fim de correr cada teste</t>
   </si>
 </sst>
 </file>
@@ -243,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,8 +283,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -622,11 +625,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -671,7 +687,58 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -680,6 +747,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -699,112 +820,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,11 +1164,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1191,11 +1228,11 @@
       <c r="A9" s="33">
         <v>1</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="24" t="s">
         <v>2</v>
       </c>
@@ -1210,12 +1247,12 @@
       <c r="A10" s="33">
         <v>2</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="44" t="s">
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="79" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="22" t="s">
@@ -1224,35 +1261,35 @@
       <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="43"/>
+      <c r="H10" s="78"/>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>3</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="45"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="80"/>
       <c r="F11" s="22" t="s">
         <v>15</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="43"/>
+      <c r="H11" s="78"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
         <v>4</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="54"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="21" t="s">
         <v>36</v>
       </c>
@@ -1268,11 +1305,11 @@
       <c r="A13" s="33">
         <v>5</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="24" t="s">
         <v>2</v>
       </c>
@@ -1287,11 +1324,11 @@
       <c r="A14" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="77"/>
       <c r="E14" s="24" t="s">
         <v>2</v>
       </c>
@@ -1303,14 +1340,14 @@
       </c>
     </row>
     <row r="15" spans="1:8" s="31" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="80"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="74"/>
       <c r="E15" s="30" t="s">
         <v>5</v>
       </c>
@@ -1325,11 +1362,11 @@
       <c r="A16" s="33">
         <v>6</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="24" t="s">
         <v>5</v>
       </c>
@@ -1344,11 +1381,11 @@
       <c r="A17" s="33">
         <v>7</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="24" t="s">
         <v>5</v>
       </c>
@@ -1363,11 +1400,11 @@
       <c r="A18" s="26">
         <v>8</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="30" t="s">
         <v>7</v>
       </c>
@@ -1379,33 +1416,31 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="81">
+        <v>9</v>
+      </c>
+      <c r="B19" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="36" t="s">
+      <c r="C19" s="83"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>16</v>
+      <c r="F19" s="86" t="s">
+        <v>15</v>
       </c>
       <c r="G19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
-        <v>9</v>
-      </c>
-      <c r="B20" s="52" t="s">
+      <c r="A20" s="33"/>
+      <c r="B20" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="21" t="s">
         <v>5</v>
       </c>
@@ -1420,11 +1455,11 @@
       <c r="A21" s="17">
         <v>10</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="7"/>
       <c r="F21" s="29"/>
     </row>
@@ -1432,11 +1467,11 @@
       <c r="A22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
       <c r="E22" s="25" t="s">
         <v>5</v>
       </c>
@@ -1451,11 +1486,11 @@
       <c r="A23" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="21" t="s">
         <v>36</v>
       </c>
@@ -1470,11 +1505,11 @@
       <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47"/>
       <c r="E24" s="7"/>
       <c r="F24" s="12" t="s">
         <v>14</v>
@@ -1487,23 +1522,28 @@
       <c r="A25" s="17">
         <v>11</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="59"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="29"/>
+      <c r="F25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="63"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="7"/>
       <c r="F26" s="12" t="s">
         <v>14</v>
@@ -1516,11 +1556,11 @@
       <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="63"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
       <c r="E27" s="7"/>
       <c r="F27" s="12" t="s">
         <v>14</v>
@@ -1530,17 +1570,19 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="12" t="s">
-        <v>14</v>
+      <c r="C28" s="89"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="G28" t="s">
         <v>26</v>
@@ -1550,11 +1592,11 @@
       <c r="A29" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="69"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="7"/>
       <c r="F29" s="12" t="s">
         <v>14</v>
@@ -1567,11 +1609,11 @@
       <c r="A30" s="34">
         <v>12</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="66"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="19"/>
       <c r="F30" s="12" t="s">
         <v>14</v>
@@ -1584,11 +1626,11 @@
       <c r="A31" s="17">
         <v>13</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
       <c r="E31" s="7"/>
       <c r="F31" s="29"/>
     </row>
@@ -1596,11 +1638,11 @@
       <c r="A32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="54"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="44"/>
       <c r="E32" s="25" t="s">
         <v>5</v>
       </c>
@@ -1615,11 +1657,11 @@
       <c r="A33" s="33">
         <v>14</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="54"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="44"/>
       <c r="E33" s="21" t="s">
         <v>2</v>
       </c>
@@ -1634,11 +1676,11 @@
       <c r="A34" s="33">
         <v>15</v>
       </c>
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="53"/>
-      <c r="D34" s="54"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="44"/>
       <c r="E34" s="24" t="s">
         <v>5</v>
       </c>
@@ -1653,11 +1695,11 @@
       <c r="A35" s="32">
         <v>16</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="57"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
       <c r="E35" s="8"/>
       <c r="F35" s="10"/>
       <c r="G35" t="s">
@@ -1668,11 +1710,11 @@
       <c r="A36" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="54"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="44"/>
       <c r="E36" s="25" t="s">
         <v>2</v>
       </c>
@@ -1688,11 +1730,11 @@
       <c r="A37" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="76"/>
-      <c r="D37" s="77"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="71"/>
       <c r="E37" s="8"/>
       <c r="F37" s="10"/>
       <c r="G37" s="31" t="s">
@@ -1704,11 +1746,11 @@
       <c r="A38" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="76"/>
-      <c r="D38" s="77"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="71"/>
       <c r="E38" s="8"/>
       <c r="F38" s="10"/>
       <c r="G38" s="31" t="s">
@@ -1720,11 +1762,11 @@
       <c r="A39" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="76"/>
-      <c r="D39" s="77"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="71"/>
       <c r="E39" s="8"/>
       <c r="F39" s="10"/>
       <c r="G39" s="31" t="s">
@@ -1736,11 +1778,11 @@
       <c r="A40" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="76"/>
-      <c r="D40" s="77"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
       <c r="E40" s="8"/>
       <c r="F40" s="10"/>
       <c r="G40" s="31" t="s">
@@ -1766,40 +1808,55 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="58"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="60"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="68"/>
       <c r="E42" s="8"/>
       <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="58"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="60"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="68"/>
       <c r="E43" s="8"/>
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="58"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="60"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="68"/>
       <c r="E44" s="8"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="46"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="48"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="62"/>
       <c r="E45" s="9"/>
       <c r="F45" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B28:D28"/>
@@ -1814,26 +1871,11 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>

<commit_message>
Ficheiro Excel actualizado tarefas
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
   <si>
     <t>Tarefa</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Fazer janela de Inicio para sincronizar dados pela primeira vez, e depois nas proxima vez trabalhar sempre offine</t>
+  </si>
+  <si>
+    <t>Replicar tabela de Disicplinas e metodos relativa as mesmas</t>
+  </si>
+  <si>
+    <t>Corrigido erro</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,7 +303,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -735,11 +747,147 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -748,6 +896,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -767,141 +924,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -911,16 +933,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,7 +1005,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1016,7 +1040,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1225,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,11 +1268,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1320,11 +1344,11 @@
       <c r="A9" s="19">
         <v>1</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="56"/>
       <c r="E9" s="15" t="s">
         <v>2</v>
       </c>
@@ -1341,12 +1365,12 @@
         <f>A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="57" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="52" t="s">
         <v>64</v>
       </c>
       <c r="F10" s="25" t="s">
@@ -1355,39 +1379,39 @@
       <c r="G10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="55" t="s">
+      <c r="H10" s="50" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
-        <f t="shared" ref="A11:A66" si="0">A10+1</f>
+        <f t="shared" ref="A11:A67" si="0">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="58"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="53"/>
       <c r="F11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="56"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="13" t="s">
         <v>27</v>
       </c>
@@ -1404,11 +1428,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="15" t="s">
         <v>2</v>
       </c>
@@ -1425,11 +1449,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="103"/>
       <c r="E14" s="15" t="s">
         <v>2</v>
       </c>
@@ -1446,11 +1470,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="106"/>
+      <c r="C15" s="96"/>
+      <c r="D15" s="97"/>
       <c r="E15" s="7"/>
       <c r="F15" s="29" t="s">
         <v>14</v>
@@ -1465,11 +1489,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="15" t="s">
         <v>5</v>
       </c>
@@ -1486,11 +1510,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="15" t="s">
         <v>5</v>
       </c>
@@ -1507,11 +1531,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="84"/>
-      <c r="D18" s="85"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="17" t="s">
         <v>7</v>
       </c>
@@ -1528,11 +1552,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="100"/>
       <c r="E19" s="20" t="s">
         <v>2</v>
       </c>
@@ -1549,11 +1573,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="61"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
       <c r="E20" s="13" t="s">
         <v>5</v>
       </c>
@@ -1570,11 +1594,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="67"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="7"/>
       <c r="F21" s="28"/>
       <c r="G21" s="30"/>
@@ -1585,11 +1609,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
       <c r="E22" s="16" t="s">
         <v>5</v>
       </c>
@@ -1608,11 +1632,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="61"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="13" t="s">
         <v>27</v>
       </c>
@@ -1629,11 +1653,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="73"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="7"/>
       <c r="F24" s="29" t="s">
         <v>14</v>
@@ -1648,11 +1672,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="73"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
       <c r="E25" s="7"/>
       <c r="F25" s="29" t="s">
         <v>14</v>
@@ -1667,85 +1691,90 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="95"/>
-      <c r="D26" s="96"/>
-      <c r="E26" s="41" t="s">
+      <c r="C26" s="82"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="43" t="s">
+      <c r="F26" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="44"/>
+      <c r="H26" s="48"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="45" t="s">
+      <c r="C27" s="93"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="43" t="s">
+      <c r="F27" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="44"/>
+      <c r="H27" s="48" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="19"/>
+      <c r="B28" s="107" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="108"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="111" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="112"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
         <f>A27+1</f>
         <v>20</v>
       </c>
-      <c r="B28" s="91" t="s">
+      <c r="B29" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="92"/>
-      <c r="D28" s="93"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="29" t="s">
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G29" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="30"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B30" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B30" s="66"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68"/>
       <c r="E30" s="7"/>
       <c r="F30" s="28"/>
       <c r="G30" s="30"/>
@@ -1756,20 +1785,14 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B31" s="100" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="102"/>
-      <c r="E31" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="B31" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="30"/>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1777,11 +1800,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B32" s="100" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="101"/>
-      <c r="D32" s="102"/>
+      <c r="B32" s="104" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="105"/>
+      <c r="D32" s="106"/>
       <c r="E32" s="17" t="s">
         <v>2</v>
       </c>
@@ -1798,13 +1821,13 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B33" s="100" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="102"/>
-      <c r="E33" s="103" t="s">
-        <v>5</v>
+      <c r="B33" s="104" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="105"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="17" t="s">
+        <v>2</v>
       </c>
       <c r="F33" s="26" t="s">
         <v>16</v>
@@ -1819,12 +1842,12 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B34" s="100" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="101"/>
-      <c r="D34" s="102"/>
-      <c r="E34" s="103" t="s">
+      <c r="B34" s="104" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="105"/>
+      <c r="D34" s="106"/>
+      <c r="E34" s="41" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="26" t="s">
@@ -1840,14 +1863,16 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B35" s="97" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="98"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="29" t="s">
-        <v>14</v>
+      <c r="B35" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="105"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>16</v>
       </c>
       <c r="G35" s="30" t="s">
         <v>28</v>
@@ -1859,11 +1884,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B36" s="97" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="98"/>
-      <c r="D36" s="99"/>
+      <c r="B36" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="85"/>
+      <c r="D36" s="86"/>
       <c r="E36" s="8"/>
       <c r="F36" s="29" t="s">
         <v>14</v>
@@ -1878,11 +1903,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B37" s="97" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="98"/>
-      <c r="D37" s="99"/>
+      <c r="B37" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="85"/>
+      <c r="D37" s="86"/>
       <c r="E37" s="8"/>
       <c r="F37" s="29" t="s">
         <v>14</v>
@@ -1897,11 +1922,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B38" s="97" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="98"/>
-      <c r="D38" s="99"/>
+      <c r="B38" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="85"/>
+      <c r="D38" s="86"/>
       <c r="E38" s="8"/>
       <c r="F38" s="29" t="s">
         <v>14</v>
@@ -1916,12 +1941,18 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B39" s="74"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="76"/>
+      <c r="B39" s="84" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="85"/>
+      <c r="D39" s="86"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
+      <c r="F39" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,9 +1960,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="73"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
       <c r="E40" s="8"/>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
@@ -1942,9 +1973,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="73"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="68"/>
       <c r="E41" s="8"/>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
@@ -1955,10 +1986,10 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="7"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="8"/>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
       <c r="H42" s="10"/>
@@ -1968,18 +1999,12 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B43" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="78"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="30" t="s">
-        <v>45</v>
-      </c>
+      <c r="B43" s="75"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1987,14 +2012,18 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B44" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="66"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="30"/>
+      <c r="B44" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="73"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>45</v>
+      </c>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2002,20 +2031,14 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B45" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="60"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="30" t="s">
-        <v>21</v>
-      </c>
+      <c r="B45" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="61"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="30"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2023,12 +2046,20 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B46" s="74"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="37"/>
+      <c r="B46" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="55"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2036,9 +2067,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B47" s="74"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="76"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="71"/>
       <c r="E47" s="14"/>
       <c r="F47" s="31"/>
       <c r="G47" s="37"/>
@@ -2049,9 +2080,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B48" s="74"/>
-      <c r="C48" s="75"/>
-      <c r="D48" s="76"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="71"/>
       <c r="E48" s="14"/>
       <c r="F48" s="31"/>
       <c r="G48" s="37"/>
@@ -2062,9 +2093,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B49" s="74"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="76"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="71"/>
       <c r="E49" s="14"/>
       <c r="F49" s="31"/>
       <c r="G49" s="37"/>
@@ -2075,20 +2106,12 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B50" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="60"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" s="30" t="s">
-        <v>21</v>
-      </c>
+      <c r="B50" s="69"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="37"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2096,45 +2119,53 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B51" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="60"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="15" t="s">
-        <v>5</v>
+      <c r="B51" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="55"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="F51" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="38" t="s">
+      <c r="G51" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="35" t="s">
-        <v>41</v>
-      </c>
+      <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B52" s="68"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="10"/>
+      <c r="B52" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="55"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="35" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B53" s="68"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="70"/>
+      <c r="B53" s="63"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="65"/>
       <c r="E53" s="8"/>
       <c r="F53" s="30"/>
       <c r="G53" s="30"/>
@@ -2145,9 +2176,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B54" s="68"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="70"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="65"/>
       <c r="E54" s="8"/>
       <c r="F54" s="30"/>
       <c r="G54" s="30"/>
@@ -2158,16 +2189,12 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B55" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="C55" s="69"/>
-      <c r="D55" s="70"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="64"/>
+      <c r="D55" s="65"/>
       <c r="E55" s="8"/>
       <c r="F55" s="30"/>
-      <c r="G55" s="30" t="s">
-        <v>21</v>
-      </c>
+      <c r="G55" s="30"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2175,38 +2202,36 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B56" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="60"/>
-      <c r="D56" s="61"/>
-      <c r="E56" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F56" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G56" s="37" t="s">
+      <c r="B56" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="64"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H56" s="21"/>
+      <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B57" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="75"/>
-      <c r="D57" s="76"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" s="30" t="s">
-        <v>28</v>
+      <c r="B57" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="55"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>21</v>
       </c>
       <c r="H57" s="21"/>
     </row>
@@ -2215,11 +2240,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B58" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="75"/>
-      <c r="D58" s="76"/>
+      <c r="B58" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="70"/>
+      <c r="D58" s="71"/>
       <c r="E58" s="8"/>
       <c r="F58" s="29" t="s">
         <v>14</v>
@@ -2234,11 +2259,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B59" s="74" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="75"/>
-      <c r="D59" s="76"/>
+      <c r="B59" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="70"/>
+      <c r="D59" s="71"/>
       <c r="E59" s="8"/>
       <c r="F59" s="29" t="s">
         <v>14</v>
@@ -2253,11 +2278,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B60" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60" s="75"/>
-      <c r="D60" s="76"/>
+      <c r="B60" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="70"/>
+      <c r="D60" s="71"/>
       <c r="E60" s="8"/>
       <c r="F60" s="29" t="s">
         <v>14</v>
@@ -2272,11 +2297,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B61" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" s="75"/>
-      <c r="D61" s="76"/>
+      <c r="B61" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="70"/>
+      <c r="D61" s="71"/>
       <c r="E61" s="8"/>
       <c r="F61" s="29" t="s">
         <v>14</v>
@@ -2291,11 +2316,11 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B62" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="C62" s="72"/>
-      <c r="D62" s="73"/>
+      <c r="B62" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="70"/>
+      <c r="D62" s="71"/>
       <c r="E62" s="8"/>
       <c r="F62" s="29" t="s">
         <v>14</v>
@@ -2303,19 +2328,25 @@
       <c r="G62" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H62" s="10"/>
+      <c r="H62" s="21"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B63" s="71"/>
-      <c r="C63" s="72"/>
-      <c r="D63" s="73"/>
+      <c r="B63" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="67"/>
+      <c r="D63" s="68"/>
       <c r="E63" s="8"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
+      <c r="F63" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2323,9 +2354,9 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B64" s="71"/>
-      <c r="C64" s="72"/>
-      <c r="D64" s="73"/>
+      <c r="B64" s="66"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="68"/>
       <c r="E64" s="8"/>
       <c r="F64" s="30"/>
       <c r="G64" s="30"/>
@@ -2336,62 +2367,85 @@
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="66"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B66" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="72"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="29" t="s">
+      <c r="C66" s="67"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="30" t="s">
+      <c r="G66" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H65" s="10" t="s">
+      <c r="H66" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B66" s="62"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="11"/>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B67" s="57"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B32:D32"/>
+  <mergeCells count="60">
+    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B16:D16"/>
     <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B42:D42"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B17:D17"/>
@@ -2399,35 +2453,24 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B61:D61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>

<commit_message>
Apresentação para a aula teórica 16-05-2014, actualização de tarefas.xls, e "piquenos" ajustes nos layouts
</commit_message>
<xml_diff>
--- a/Tarefas_app.xlsx
+++ b/Tarefas_app.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Folha2" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="74">
   <si>
     <t>Tarefa</t>
   </si>
@@ -223,6 +223,21 @@
   </si>
   <si>
     <t>Corrigido erro</t>
+  </si>
+  <si>
+    <t>Luis Amendoeira.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Na execução sequencial do teste este verifica automaticamente qual o tipo e escolhe o layout adequado</t>
+  </si>
+  <si>
+    <t>Implementar Multi-ecrãs</t>
+  </si>
+  <si>
+    <t>Suspenso</t>
   </si>
 </sst>
 </file>
@@ -703,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -762,177 +777,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -945,6 +789,175 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,7 +1018,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1040,7 +1053,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1251,16 +1264,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="18" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
@@ -1268,11 +1281,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1344,11 +1357,11 @@
       <c r="A9" s="19">
         <v>1</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="15" t="s">
         <v>2</v>
       </c>
@@ -1365,12 +1378,12 @@
         <f>A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="52" t="s">
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="102" t="s">
         <v>64</v>
       </c>
       <c r="F10" s="25" t="s">
@@ -1379,7 +1392,7 @@
       <c r="G10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="100" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1388,30 +1401,30 @@
         <f t="shared" ref="A11:A67" si="0">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="53"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="103"/>
       <c r="F11" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="51"/>
+      <c r="H11" s="101"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="13" t="s">
         <v>27</v>
       </c>
@@ -1428,11 +1441,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="15" t="s">
         <v>2</v>
       </c>
@@ -1449,11 +1462,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="102"/>
-      <c r="D14" s="103"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="87"/>
       <c r="E14" s="15" t="s">
         <v>2</v>
       </c>
@@ -1470,16 +1483,18 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="96"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="30" t="s">
+      <c r="C15" s="113"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H15" s="34"/>
@@ -1489,11 +1504,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="56"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="78"/>
       <c r="E16" s="15" t="s">
         <v>5</v>
       </c>
@@ -1510,11 +1525,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="15" t="s">
         <v>5</v>
       </c>
@@ -1531,18 +1546,18 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="80"/>
+      <c r="C18" s="98"/>
+      <c r="D18" s="99"/>
       <c r="E18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="38" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="10"/>
@@ -1552,11 +1567,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="100"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="20" t="s">
         <v>2</v>
       </c>
@@ -1573,11 +1588,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="56"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="13" t="s">
         <v>5</v>
       </c>
@@ -1594,11 +1609,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="90"/>
       <c r="E21" s="7"/>
       <c r="F21" s="28"/>
       <c r="G21" s="30"/>
@@ -1609,11 +1624,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="78"/>
       <c r="E22" s="16" t="s">
         <v>5</v>
       </c>
@@ -1632,11 +1647,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="56"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="13" t="s">
         <v>27</v>
       </c>
@@ -1653,16 +1668,16 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
       <c r="E24" s="7"/>
       <c r="F24" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="111" t="s">
         <v>28</v>
       </c>
       <c r="H24" s="10"/>
@@ -1672,16 +1687,18 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="30" t="s">
+      <c r="C25" s="77"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="109" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="10"/>
@@ -1691,11 +1708,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="83"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="45" t="s">
         <v>27</v>
       </c>
@@ -1712,11 +1729,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="94"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
       <c r="E27" s="49" t="s">
         <v>27</v>
       </c>
@@ -1731,27 +1748,30 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="107" t="s">
+      <c r="A28" s="19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="110" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="111" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="111" t="s">
+      <c r="F28" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="112"/>
+      <c r="H28" s="55"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
-        <f>A27+1</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>47</v>
@@ -1762,261 +1782,275 @@
       <c r="F29" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="111" t="s">
         <v>28</v>
       </c>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="68"/>
+      <c r="A30" s="19">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="68"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
       <c r="E30" s="7"/>
       <c r="F30" s="28"/>
       <c r="G30" s="30"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B31" s="60" t="s">
+      <c r="A31" s="19">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B31" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="62"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
       <c r="E31" s="7"/>
       <c r="F31" s="28"/>
       <c r="G31" s="30"/>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B32" s="104" t="s">
+      <c r="A32" s="19">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B32" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="105"/>
-      <c r="D32" s="106"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="61"/>
       <c r="E32" s="17" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="30" t="s">
+      <c r="G32" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B33" s="104" t="s">
+      <c r="A33" s="19">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B33" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="105"/>
-      <c r="D33" s="106"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="61"/>
       <c r="E33" s="17" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="F33" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="30" t="s">
+      <c r="G33" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B34" s="104" t="s">
+      <c r="A34" s="19">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B34" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="105"/>
-      <c r="D34" s="106"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="41" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B35" s="104" t="s">
+      <c r="A35" s="19">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B35" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="105"/>
-      <c r="D35" s="106"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="61"/>
       <c r="E35" s="41" t="s">
         <v>5</v>
       </c>
       <c r="F35" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B36" s="84" t="s">
+      <c r="A36" s="19">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B36" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="85"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="30" t="s">
+      <c r="C36" s="60"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="107" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B37" s="84" t="s">
+      <c r="A37" s="19">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B37" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="85"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="30" t="s">
+      <c r="C37" s="60"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="107" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B38" s="84" t="s">
+      <c r="A38" s="19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B38" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="85"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="30" t="s">
+      <c r="C38" s="60"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B39" s="84" t="s">
+      <c r="A39" s="19">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B39" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="85"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="30" t="s">
+      <c r="C39" s="60"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="38" t="s">
         <v>28</v>
       </c>
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B40" s="69"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="71"/>
+      <c r="A40" s="19">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B40" s="56"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="58"/>
       <c r="E40" s="8"/>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B41" s="66"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="68"/>
+      <c r="A41" s="19">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="69"/>
+      <c r="D41" s="70"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
+      <c r="F41" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="111" t="s">
+        <v>45</v>
+      </c>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="68"/>
+      <c r="A42" s="19">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B42" s="68"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="8"/>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="77"/>
+      <c r="A43" s="19">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B43" s="94"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="96"/>
       <c r="E43" s="7"/>
       <c r="F43" s="30"/>
       <c r="G43" s="30"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B44" s="72" t="s">
+      <c r="A44" s="19">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B44" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="73"/>
-      <c r="D44" s="74"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="93"/>
       <c r="E44" s="12"/>
       <c r="F44" s="29" t="s">
         <v>14</v>
@@ -2027,124 +2061,124 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B45" s="60" t="s">
+      <c r="A45" s="19">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B45" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="90"/>
       <c r="E45" s="7"/>
       <c r="F45" s="28"/>
       <c r="G45" s="30"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B46" s="54" t="s">
+      <c r="A46" s="19">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B46" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="78"/>
       <c r="E46" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F46" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G46" s="30" t="s">
+      <c r="G46" s="109" t="s">
         <v>21</v>
       </c>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B47" s="69"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="71"/>
+      <c r="A47" s="19">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B47" s="56"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="58"/>
       <c r="E47" s="14"/>
       <c r="F47" s="31"/>
       <c r="G47" s="37"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B48" s="69"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="71"/>
+      <c r="A48" s="19">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B48" s="56"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="58"/>
       <c r="E48" s="14"/>
       <c r="F48" s="31"/>
       <c r="G48" s="37"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B49" s="69"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="71"/>
+      <c r="A49" s="19">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B49" s="56"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="58"/>
       <c r="E49" s="14"/>
       <c r="F49" s="31"/>
       <c r="G49" s="37"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B50" s="69"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="71"/>
+      <c r="A50" s="19">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B50" s="56"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="58"/>
       <c r="E50" s="14"/>
       <c r="F50" s="31"/>
       <c r="G50" s="37"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B51" s="54" t="s">
+      <c r="A51" s="19">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B51" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="55"/>
-      <c r="D51" s="56"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="78"/>
       <c r="E51" s="13" t="s">
         <v>2</v>
       </c>
       <c r="F51" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="30" t="s">
+      <c r="G51" s="109" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B52" s="54" t="s">
+      <c r="A52" s="19">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B52" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="55"/>
-      <c r="D52" s="56"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="78"/>
       <c r="E52" s="15" t="s">
         <v>5</v>
       </c>
@@ -2155,58 +2189,58 @@
         <v>21</v>
       </c>
       <c r="H52" s="35" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B53" s="63"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="65"/>
+      <c r="A53" s="19">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B53" s="62"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="64"/>
       <c r="E53" s="8"/>
       <c r="F53" s="30"/>
       <c r="G53" s="30"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B54" s="63"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="65"/>
+      <c r="A54" s="19">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B54" s="62"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="64"/>
       <c r="E54" s="8"/>
       <c r="F54" s="30"/>
       <c r="G54" s="30"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B55" s="63"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="65"/>
+      <c r="A55" s="19">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B55" s="62"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="64"/>
       <c r="E55" s="8"/>
       <c r="F55" s="30"/>
       <c r="G55" s="30"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B56" s="63" t="s">
+      <c r="A56" s="19">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B56" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="64"/>
-      <c r="D56" s="65"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="64"/>
       <c r="E56" s="8"/>
       <c r="F56" s="30"/>
       <c r="G56" s="30" t="s">
@@ -2215,176 +2249,190 @@
       <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B57" s="54" t="s">
+      <c r="A57" s="19">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B57" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="55"/>
-      <c r="D57" s="56"/>
+      <c r="C57" s="77"/>
+      <c r="D57" s="78"/>
       <c r="E57" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F57" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G57" s="37" t="s">
+      <c r="G57" s="109" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="21"/>
     </row>
     <row r="58" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B58" s="69" t="s">
+      <c r="A58" s="19">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B58" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="70"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="29" t="s">
+      <c r="C58" s="98"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="107" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="H58" s="21"/>
+    </row>
+    <row r="59" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="19">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B59" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="77"/>
+      <c r="D59" s="78"/>
+      <c r="E59" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="30" t="s">
+      <c r="G59" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="H58" s="21"/>
-    </row>
-    <row r="59" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B59" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="70"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="29" t="s">
+      <c r="H59" s="21"/>
+    </row>
+    <row r="60" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="19">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B60" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" s="77"/>
+      <c r="D60" s="78"/>
+      <c r="E60" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G59" s="30" t="s">
+      <c r="G60" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="H59" s="21"/>
-    </row>
-    <row r="60" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B60" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="70"/>
-      <c r="D60" s="71"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="29" t="s">
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="19">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B61" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="77"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="30" t="s">
+      <c r="G61" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="H60" s="21"/>
-    </row>
-    <row r="61" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B61" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="C61" s="70"/>
-      <c r="D61" s="71"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="29" t="s">
+      <c r="H61" s="21"/>
+    </row>
+    <row r="62" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="19">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B62" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="77"/>
+      <c r="D62" s="78"/>
+      <c r="E62" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G62" s="109" t="s">
+        <v>23</v>
+      </c>
+      <c r="H62" s="110" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="19">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B63" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="77"/>
+      <c r="D63" s="78"/>
+      <c r="E63" s="108" t="s">
+        <v>2</v>
+      </c>
+      <c r="F63" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G61" s="30" t="s">
+      <c r="G63" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="H61" s="21"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B62" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="70"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H62" s="21"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B63" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="67"/>
-      <c r="D63" s="68"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" s="30" t="s">
-        <v>28</v>
-      </c>
       <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B64" s="66"/>
-      <c r="C64" s="67"/>
-      <c r="D64" s="68"/>
+      <c r="A64" s="19">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B64" s="68"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="70"/>
       <c r="E64" s="8"/>
       <c r="F64" s="30"/>
       <c r="G64" s="30"/>
       <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B65" s="66"/>
-      <c r="C65" s="67"/>
-      <c r="D65" s="68"/>
+      <c r="A65" s="19">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B65" s="68"/>
+      <c r="C65" s="69"/>
+      <c r="D65" s="70"/>
       <c r="E65" s="8"/>
       <c r="F65" s="30"/>
       <c r="G65" s="30"/>
       <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B66" s="66" t="s">
+      <c r="A66" s="19">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B66" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C66" s="67"/>
-      <c r="D66" s="68"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="70"/>
       <c r="E66" s="14"/>
       <c r="F66" s="29" t="s">
         <v>14</v>
@@ -2397,13 +2445,13 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="19" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="B67" s="57"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="59"/>
+      <c r="A67" s="19">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B67" s="104"/>
+      <c r="C67" s="105"/>
+      <c r="D67" s="106"/>
       <c r="E67" s="9"/>
       <c r="F67" s="32"/>
       <c r="G67" s="32"/>
@@ -2411,19 +2459,37 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B39:D39"/>
@@ -2440,37 +2506,19 @@
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>